<commit_message>
Finished designing the map
</commit_message>
<xml_diff>
--- a/level.xlsx
+++ b/level.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17814\Documents\GitHub\Shop Sim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7BD15C-1605-44C7-A757-A22C666AD20E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52828E9-4434-413C-BF48-B71843E201FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AA1B69AA-641A-4C67-8795-AA8A2387FE59}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.5546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -577,7 +577,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="2"/>
+      <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="2"/>
     </row>
@@ -593,7 +593,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="2"/>
+      <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="2"/>

</xml_diff>

<commit_message>
Currently has a working dictionary storing blockID and times visited
</commit_message>
<xml_diff>
--- a/level.xlsx
+++ b/level.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17814\Documents\GitHub\Shop Sim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52828E9-4434-413C-BF48-B71843E201FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169ACFD2-6CED-4D54-8022-04805E714CDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AA1B69AA-641A-4C67-8795-AA8A2387FE59}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="2">
   <si>
     <t>入口</t>
   </si>
@@ -420,134 +420,271 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5942B945-C913-4C72-BEA4-C367E9623B99}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:AJ15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.5546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="4"/>
       <c r="O1" s="2"/>
-    </row>
-    <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V1" s="2"/>
+      <c r="W1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="4"/>
+      <c r="AG1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI1" s="4"/>
+      <c r="AJ1" s="2"/>
+    </row>
+    <row r="2" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="4"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
+      <c r="N2" s="4"/>
       <c r="O2" s="2"/>
-    </row>
-    <row r="3" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V2" s="2"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="2"/>
+    </row>
+    <row r="3" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="1"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="1"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="2"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
+      <c r="N3" s="4"/>
       <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V3" s="2"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="2"/>
+    </row>
+    <row r="4" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="1"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="1"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="2"/>
+      <c r="K4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
+      <c r="N4" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V4" s="2"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="2"/>
+    </row>
+    <row r="5" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="1"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
       <c r="J5" s="2"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="2"/>
+      <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="2"/>
-    </row>
-    <row r="6" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V5" s="2"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1"/>
+      <c r="AJ5" s="2"/>
+    </row>
+    <row r="6" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="2"/>
+      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="1"/>
+      <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="1"/>
+      <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="1"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="1"/>
+      <c r="M6" s="2"/>
       <c r="N6" s="1"/>
       <c r="O6" s="2"/>
-    </row>
-    <row r="7" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V6" s="2"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="2"/>
+    </row>
+    <row r="7" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="2"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="2"/>
+      <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="1"/>
+      <c r="M7" s="2"/>
       <c r="N7" s="1"/>
       <c r="O7" s="2"/>
-    </row>
-    <row r="8" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V7" s="2"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="1"/>
+      <c r="AJ7" s="2"/>
+    </row>
+    <row r="8" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -563,141 +700,245 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="2"/>
-    </row>
-    <row r="9" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V8" s="2"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="2"/>
+    </row>
+    <row r="9" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="2"/>
+      <c r="C9" s="1"/>
       <c r="D9" s="2"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="2"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="2"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="J9" s="2"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="L9" s="2"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="2"/>
-    </row>
-    <row r="10" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V9" s="2"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
+      <c r="AJ9" s="2"/>
+    </row>
+    <row r="10" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
+      <c r="C10" s="1"/>
       <c r="D10" s="2"/>
       <c r="E10" s="1"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="G10" s="1"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="I10" s="1"/>
       <c r="J10" s="2"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
+      <c r="L10" s="2"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="2"/>
-    </row>
-    <row r="11" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V10" s="2"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="2"/>
+    </row>
+    <row r="11" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="D11" s="2"/>
       <c r="E11" s="1"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="1"/>
       <c r="J11" s="2"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="L11" s="2"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="2"/>
-    </row>
-    <row r="12" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V11" s="2"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="2"/>
+      <c r="AH11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="2"/>
+    </row>
+    <row r="12" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
-      <c r="B12" s="4"/>
+      <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="4"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="1"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="1"/>
       <c r="J12" s="2"/>
       <c r="K12" s="1"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
+      <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="2"/>
-    </row>
-    <row r="13" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V12" s="2"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="2"/>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="1"/>
+      <c r="AJ12" s="2"/>
+    </row>
+    <row r="13" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
-      <c r="B13" s="4"/>
+      <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="4"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="1"/>
       <c r="J13" s="2"/>
       <c r="K13" s="1"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
+      <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="2"/>
-    </row>
-    <row r="14" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V13" s="2"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="2"/>
+      <c r="AH13" s="1"/>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="2"/>
+    </row>
+    <row r="14" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
-      <c r="B14" s="4"/>
+      <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="2"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="2"/>
-    </row>
-    <row r="15" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V14" s="2"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1"/>
+      <c r="AI14" s="1"/>
+      <c r="AJ14" s="2"/>
+    </row>
+    <row r="15" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="B15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
       <c r="O15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2"/>
+      <c r="AF15" s="2"/>
+      <c r="AG15" s="2"/>
+      <c r="AH15" s="2"/>
+      <c r="AI15" s="2"/>
+      <c r="AJ15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>